<commit_message>
sek, seng bener seng iki
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07250964-3238-4241-8FD9-D2190020E525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC3772-FE80-7042-8919-02C3BB515715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14060" xr2:uid="{329E2B7B-EBAD-E649-85EA-0820AD4453A7}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="66">
   <si>
     <t>HIB</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>NQ908B</t>
+  </si>
+  <si>
+    <t>JL01-8389</t>
+  </si>
+  <si>
+    <t>TGBU6779091</t>
   </si>
 </sst>
 </file>
@@ -700,6 +706,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -2062,7 +2070,7 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
@@ -2088,7 +2096,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="P25" s="6">
         <v>20190705</v>
@@ -2117,7 +2125,7 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
@@ -2143,7 +2151,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="P26" s="6">
         <v>20190705</v>

</xml_diff>

<commit_message>
db baru lagi, maaf banyak refisi data inputnya. sebel gw
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC3772-FE80-7042-8919-02C3BB515715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07250964-3238-4241-8FD9-D2190020E525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14060" xr2:uid="{329E2B7B-EBAD-E649-85EA-0820AD4453A7}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="64">
   <si>
     <t>HIB</t>
   </si>
@@ -251,12 +251,6 @@
   </si>
   <si>
     <t>NQ908B</t>
-  </si>
-  <si>
-    <t>JL01-8389</t>
-  </si>
-  <si>
-    <t>TGBU6779091</t>
   </si>
 </sst>
 </file>
@@ -706,8 +700,6 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -2070,7 +2062,7 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
@@ -2096,7 +2088,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="P25" s="6">
         <v>20190705</v>
@@ -2125,7 +2117,7 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
-        <v>65</v>
+        <v>31</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
@@ -2151,7 +2143,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6" t="s">
-        <v>64</v>
+        <v>33</v>
       </c>
       <c r="P26" s="6">
         <v>20190705</v>

</xml_diff>

<commit_message>
Hahahaha, iki sek yo
</commit_message>
<xml_diff>
--- a/excel/import_data.xlsx
+++ b/excel/import_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/fa_sai/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07250964-3238-4241-8FD9-D2190020E525}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AC3772-FE80-7042-8919-02C3BB515715}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="960" windowWidth="25040" windowHeight="14060" xr2:uid="{329E2B7B-EBAD-E649-85EA-0820AD4453A7}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="66">
   <si>
     <t>HIB</t>
   </si>
@@ -251,6 +251,12 @@
   </si>
   <si>
     <t>NQ908B</t>
+  </si>
+  <si>
+    <t>JL01-8389</t>
+  </si>
+  <si>
+    <t>TGBU6779091</t>
   </si>
 </sst>
 </file>
@@ -700,6 +706,8 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
@@ -2062,7 +2070,7 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="6" t="s">
@@ -2088,7 +2096,7 @@
       <c r="M25" s="6"/>
       <c r="N25" s="6"/>
       <c r="O25" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="P25" s="6">
         <v>20190705</v>
@@ -2117,7 +2125,7 @@
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
@@ -2143,7 +2151,7 @@
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
       <c r="O26" s="6" t="s">
-        <v>33</v>
+        <v>64</v>
       </c>
       <c r="P26" s="6">
         <v>20190705</v>

</xml_diff>